<commit_message>
Adjusted epsilon and norm of L
</commit_message>
<xml_diff>
--- a/PopulationByCountry.xlsx
+++ b/PopulationByCountry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andregerbaulet/Documents/Corona/SIR model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin/Documents/Enfidem App/Epidemic-modelling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469C80D4-BF33-C44E-84B9-A66168C644C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3DE6AF-E93C-A34A-8362-21E7D99D9EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{894A8C14-C469-7947-B8BB-D8E5FAE1679C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="476">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1455,6 +1455,12 @@
   </si>
   <si>
     <t>South Korea</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1516,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1806,10 +1812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE9617B-9A63-9F47-89B1-4E36A756A529}">
-  <dimension ref="A1:B477"/>
+  <dimension ref="A1:B478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="M382" sqref="M382"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1819,1378 +1825,1378 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>38041757</v>
+        <v>474</v>
+      </c>
+      <c r="B1" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1308064176</v>
+        <v>38041757</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1306320572</v>
+        <v>1308064176</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>1306903030</v>
+        <v>1306320572</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>154013705</v>
+        <v>1306903030</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>382531219</v>
+        <v>154013705</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>203493226</v>
+        <v>382531219</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>179956492</v>
+        <v>203493226</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>386908388</v>
+        <v>179956492</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>1150190575</v>
+        <v>386908388</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>2880913</v>
+        <v>1150190575</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>43053054</v>
+        <v>2880913</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>55312</v>
+        <v>43053054</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>111736664</v>
+        <v>55312</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>77146</v>
+        <v>111736664</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>31825299</v>
+        <v>77146</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>14872</v>
+        <v>31825299</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>97115</v>
+        <v>14872</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>44780675</v>
+        <v>97115</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>2957728</v>
+        <v>44780675</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>106310</v>
+        <v>2957728</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>4601371266</v>
+        <v>106310</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>2956245278</v>
+        <v>4601371266</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>4582136259</v>
+        <v>2956245278</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>660718726</v>
+        <v>4582136259</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>25203200</v>
+        <v>660718726</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>29986262</v>
+        <v>25203200</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>8955108</v>
+        <v>29986262</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>10047719</v>
+        <v>8955108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>3157123227</v>
+        <v>10047719</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>3215681494</v>
+        <v>3157123227</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>389486</v>
+        <v>3215681494</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>1641164</v>
+        <v>389486</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>163046173</v>
+        <v>1641164</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>287021</v>
+        <v>163046173</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>9452409</v>
+        <v>287021</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>11539326</v>
+        <v>9452409</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>390351</v>
+        <v>11539326</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>3353564722</v>
+        <v>390351</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>1164118622</v>
+        <v>3353564722</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>1552928523</v>
+        <v>1164118622</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>414572416</v>
+        <v>1552928523</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>206761581</v>
+        <v>414572416</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>15183580</v>
+        <v>206761581</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
-        <v>11801151</v>
+        <v>15183580</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
-        <v>62508</v>
+        <v>11801151</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
-        <v>763094</v>
+        <v>62508</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>342832245</v>
+        <v>763094</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>58535065</v>
+        <v>342832245</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>11513102</v>
+        <v>58535065</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>25983</v>
+        <v>11513102</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>3300998</v>
+        <v>25983</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>2303703</v>
+        <v>3300998</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
-        <v>211049519</v>
+        <v>2303703</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>30033</v>
+        <v>211049519</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
-        <v>433296</v>
+        <v>30033</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>7000117</v>
+        <v>433296</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>20321383</v>
+        <v>7000117</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>11530577</v>
+        <v>20321383</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>549936</v>
+        <v>11530577</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>16486542.000000002</v>
+        <v>549936</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>25876387</v>
+        <v>16486542.000000002</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>37411038</v>
+        <v>25876387</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>43335006</v>
+        <v>37411038</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>18669459</v>
+        <v>43335006</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>64947.999999999993</v>
+        <v>18669459</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>4745179</v>
+        <v>64947.999999999993</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>177586525</v>
+        <v>4745179</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>73212111</v>
+        <v>177586525</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>25839142</v>
+        <v>73212111</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>1991423507</v>
+        <v>25839142</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72">
-        <v>15946882</v>
+        <v>1991423507</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>172264</v>
+        <v>15946882</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>18952035</v>
+        <v>172264</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>1433783692</v>
+        <v>18952035</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>1465634176</v>
+        <v>1433783692</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>7436157</v>
+        <v>1465634176</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>640446</v>
+        <v>7436157</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>23773881</v>
+        <v>640446</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>50339443</v>
+        <v>23773881</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81">
-        <v>289579128</v>
+        <v>50339443</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82">
-        <v>2529752075</v>
+        <v>289579128</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83">
-        <v>569747835</v>
+        <v>2529752075</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84">
-        <v>1805540408</v>
+        <v>569747835</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85">
-        <v>44231064</v>
+        <v>1805540408</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>69169112</v>
+        <v>44231064</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87">
-        <v>41063656</v>
+        <v>69169112</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88">
-        <v>850891</v>
+        <v>41063656</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>5380504</v>
+        <v>850891</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90">
-        <v>17547</v>
+        <v>5380504</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>5047561</v>
+        <v>17547</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>7130128743</v>
+        <v>5047561</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>975801688</v>
+        <v>7130128743</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94">
-        <v>4437345520</v>
+        <v>975801688</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>678689328</v>
+        <v>4437345520</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>629563215</v>
+        <v>678689328</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>366600944</v>
+        <v>629563215</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>42128048</v>
+        <v>366600944</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>4130299</v>
+        <v>42128048</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>11333484</v>
+        <v>4130299</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>163423</v>
+        <v>11333484</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102">
-        <v>1198574</v>
+        <v>163423</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103">
-        <v>10689213</v>
+        <v>1198574</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104">
-        <v>25716554</v>
+        <v>10689213</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>473</v>
+        <v>103</v>
       </c>
       <c r="B105">
-        <v>25666158</v>
+        <v>25716554</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>473</v>
       </c>
       <c r="B106">
-        <v>86790568</v>
+        <v>25666158</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107">
-        <v>5771877</v>
+        <v>86790568</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108">
-        <v>5877214</v>
+        <v>5771877</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109">
-        <v>973557</v>
+        <v>5877214</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110">
-        <v>71808</v>
+        <v>973557</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111">
-        <v>10738957</v>
+        <v>71808</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112">
-        <v>366475955</v>
+        <v>10738957</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113">
-        <v>1296492596</v>
+        <v>366475955</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114">
-        <v>636072786</v>
+        <v>1296492596</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115">
-        <v>12044798</v>
+        <v>636072786</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116">
-        <v>1648837239</v>
+        <v>12044798</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117">
-        <v>236086580</v>
+        <v>1648837239</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118">
-        <v>42115282</v>
+        <v>236086580</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119">
-        <v>2001641003</v>
+        <v>42115282</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120">
-        <v>662011846</v>
+        <v>2001641003</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121">
-        <v>4029580432</v>
+        <v>662011846</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122">
-        <v>162966739</v>
+        <v>4029580432</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123">
-        <v>1792323367</v>
+        <v>162966739</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124">
-        <v>2074290326</v>
+        <v>1792323367</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125">
-        <v>660718726</v>
+        <v>2074290326</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126">
-        <v>90214320</v>
+        <v>660718726</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127">
-        <v>504210404</v>
+        <v>90214320</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128">
-        <v>4590691950</v>
+        <v>504210404</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129">
-        <v>164025746</v>
+        <v>4590691950</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130">
-        <v>310553245</v>
+        <v>164025746</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131">
-        <v>12129020</v>
+        <v>310553245</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132">
-        <v>1835297503</v>
+        <v>12129020</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133">
-        <v>223183438</v>
+        <v>1835297503</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134">
-        <v>92316630</v>
+        <v>223183438</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135">
-        <v>2387495225</v>
+        <v>92316630</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136">
-        <v>1887677496</v>
+        <v>2387495225</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137">
-        <v>4590672789</v>
+        <v>1887677496</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138">
-        <v>222610632</v>
+        <v>4590672789</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139">
-        <v>222836176</v>
+        <v>222610632</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140">
-        <v>4590691950</v>
+        <v>222836176</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141">
-        <v>1911735616</v>
+        <v>4590691950</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142">
-        <v>2073030029</v>
+        <v>1911735616</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143">
-        <v>2057885279</v>
+        <v>2073030029</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144">
-        <v>580268276</v>
+        <v>2057885279</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B145">
-        <v>197481050</v>
+        <v>580268276</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B146">
-        <v>398460423</v>
+        <v>197481050</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B147">
-        <v>1714557469</v>
+        <v>398460423</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148">
-        <v>428166389</v>
+        <v>1714557469</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149">
-        <v>93768211</v>
+        <v>428166389</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B150">
-        <v>57694359</v>
+        <v>93768211</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B151">
-        <v>97996994</v>
+        <v>57694359</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B152">
-        <v>178706825</v>
+        <v>97996994</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B153">
-        <v>367845981</v>
+        <v>178706825</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B154">
-        <v>190068644</v>
+        <v>367845981</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B155">
-        <v>433904943</v>
+        <v>190068644</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B156">
-        <v>1672611120</v>
+        <v>433904943</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B157">
-        <v>293444921</v>
+        <v>1672611120</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B158">
-        <v>340313688</v>
+        <v>293444921</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B159">
-        <v>2334622966</v>
+        <v>340313688</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B160">
-        <v>198465942</v>
+        <v>2334622966</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B161">
-        <v>386908388</v>
+        <v>198465942</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B162">
-        <v>504210404</v>
+        <v>386908388</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B163">
-        <v>17373657</v>
+        <v>504210404</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B164">
-        <v>100388076</v>
+        <v>17373657</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B165">
-        <v>6453550</v>
+        <v>100388076</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B166">
-        <v>1355982</v>
+        <v>6453550</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B167">
-        <v>3497117</v>
+        <v>1355982</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B168">
-        <v>1325649</v>
+        <v>3497117</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B169">
-        <v>1148133</v>
+        <v>1325649</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B170">
-        <v>112078727</v>
+        <v>1148133</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B171">
-        <v>222594686</v>
+        <v>112078727</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B172">
-        <v>747182815</v>
+        <v>222594686</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
@@ -3203,7 +3209,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B174">
         <v>747182815</v>
@@ -3211,522 +3217,522 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B175">
-        <v>1113783759</v>
+        <v>747182815</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B176">
-        <v>384069996</v>
+        <v>1113783759</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B177">
-        <v>14347277</v>
+        <v>384069996</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B178">
-        <v>408593654</v>
+        <v>14347277</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B179">
-        <v>512516929</v>
+        <v>408593654</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B180">
-        <v>3372</v>
+        <v>512516929</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B181">
-        <v>48677</v>
+        <v>3372</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B182">
-        <v>889955</v>
+        <v>48677</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B183">
-        <v>5532159</v>
+        <v>889955</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B184">
-        <v>65129731</v>
+        <v>5532159</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B185">
-        <v>67978398</v>
+        <v>65129731</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B186">
-        <v>290823</v>
+        <v>67978398</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B187">
-        <v>279285</v>
+        <v>290823</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B188">
-        <v>2172578</v>
+        <v>279285</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B189">
-        <v>2347696</v>
+        <v>2172578</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B190">
-        <v>3996762</v>
+        <v>2347696</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B191">
-        <v>83517046</v>
+        <v>3996762</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B192">
-        <v>30417858</v>
+        <v>83517046</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B193">
-        <v>33706</v>
+        <v>30417858</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B194">
-        <v>406373337</v>
+        <v>33706</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B195">
-        <v>10473452</v>
+        <v>406373337</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B196">
-        <v>56660</v>
+        <v>10473452</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B197">
-        <v>112002</v>
+        <v>56660</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B198">
-        <v>6060094962</v>
+        <v>112002</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B199">
-        <v>915935544</v>
+        <v>6060094962</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B200">
-        <v>770063284</v>
+        <v>915935544</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B201">
-        <v>4622853206</v>
+        <v>770063284</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B202">
-        <v>400048</v>
+        <v>4622853206</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B203">
-        <v>167295</v>
+        <v>400048</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B204">
-        <v>17581476</v>
+        <v>167295</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B205">
-        <v>12771246</v>
+        <v>17581476</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B206">
-        <v>1920917</v>
+        <v>12771246</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B207">
-        <v>57694359</v>
+        <v>1920917</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B208">
-        <v>782775</v>
+        <v>57694359</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B209">
-        <v>11263079</v>
+        <v>782775</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B210">
-        <v>1258043484</v>
+        <v>11263079</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B211">
-        <v>815</v>
+        <v>1258043484</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B212">
-        <v>9746115</v>
+        <v>815</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B213">
-        <v>9684680</v>
+        <v>9746115</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B214">
-        <v>339037</v>
+        <v>9684680</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B215">
-        <v>1366417756</v>
+        <v>339037</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B216">
-        <v>270625567</v>
+        <v>1366417756</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>472</v>
+        <v>213</v>
       </c>
       <c r="B217">
-        <v>82913893</v>
+        <v>270625567</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>214</v>
+        <v>472</v>
       </c>
       <c r="B218">
-        <v>39309789</v>
+        <v>82913893</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B219">
-        <v>4882498</v>
+        <v>39309789</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B220">
-        <v>84589</v>
+        <v>4882498</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B221">
-        <v>8519373</v>
+        <v>84589</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B222">
-        <v>60550092</v>
+        <v>8519373</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B223">
-        <v>2948277</v>
+        <v>60550092</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B224">
-        <v>126860299</v>
+        <v>2948277</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B225">
-        <v>10101697</v>
+        <v>126860299</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B226">
-        <v>18551428</v>
+        <v>10101697</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B227">
-        <v>52573967</v>
+        <v>18551428</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B228">
-        <v>117608</v>
+        <v>52573967</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B229">
-        <v>4207077</v>
+        <v>117608</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B230">
-        <v>6415851</v>
+        <v>4207077</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B231">
-        <v>332262488</v>
+        <v>6415851</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B232">
-        <v>164025746</v>
+        <v>332262488</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B233">
-        <v>6126716</v>
+        <v>164025746</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B234">
-        <v>18557741</v>
+        <v>6126716</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B235">
-        <v>583340277</v>
+        <v>18557741</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B236">
-        <v>62367586</v>
+        <v>583340277</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B237">
-        <v>520972691</v>
+        <v>62367586</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B238">
-        <v>7169456</v>
+        <v>520972691</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B239">
-        <v>648120956</v>
+        <v>7169456</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
@@ -3739,602 +3745,602 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B241">
-        <v>568696545</v>
+        <v>648120956</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B242">
-        <v>643474175</v>
+        <v>568696545</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B243">
-        <v>1906740</v>
+        <v>643474175</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B244">
-        <v>428166389</v>
+        <v>1906740</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B245">
-        <v>1033388868</v>
+        <v>428166389</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B246">
-        <v>682410622</v>
+        <v>1033388868</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B247">
-        <v>338616201</v>
+        <v>682410622</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B248">
-        <v>11263079</v>
+        <v>338616201</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B249">
-        <v>1098966</v>
+        <v>11263079</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B250">
-        <v>6855709</v>
+        <v>1098966</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B251">
-        <v>2125267</v>
+        <v>6855709</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B252">
-        <v>6442837885</v>
+        <v>2125267</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B253">
-        <v>4977203709</v>
+        <v>6442837885</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B254">
-        <v>5409449017</v>
+        <v>4977203709</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B255">
-        <v>1308064176</v>
+        <v>5409449017</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B256">
-        <v>4474510967</v>
+        <v>1308064176</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B257">
-        <v>648120956</v>
+        <v>4474510967</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B258">
-        <v>12141786</v>
+        <v>648120956</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B259">
-        <v>4937374</v>
+        <v>12141786</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B260">
-        <v>6777453</v>
+        <v>4937374</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B261">
-        <v>38020</v>
+        <v>6777453</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B262">
-        <v>2759631</v>
+        <v>38020</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B263">
-        <v>755849741</v>
+        <v>2759631</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B264">
-        <v>3057708884</v>
+        <v>755849741</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B265">
-        <v>615730</v>
+        <v>3057708884</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B266">
-        <v>26969306</v>
+        <v>615730</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B267">
-        <v>18628749</v>
+        <v>26969306</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B268">
-        <v>31949789</v>
+        <v>18628749</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B269">
-        <v>530957</v>
+        <v>31949789</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B270">
-        <v>19658023</v>
+        <v>530957</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B271">
-        <v>440377</v>
+        <v>19658023</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B272">
-        <v>58791</v>
+        <v>440377</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B273">
-        <v>375557</v>
+        <v>58791</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B274">
-        <v>4525698</v>
+        <v>375557</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B275">
-        <v>1269670</v>
+        <v>4525698</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B276">
-        <v>266153</v>
+        <v>1269670</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B277">
-        <v>10918534</v>
+        <v>266153</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B278">
-        <v>127575529</v>
+        <v>10918534</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B279">
-        <v>543483</v>
+        <v>127575529</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B280">
-        <v>113811</v>
+        <v>543483</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B281">
-        <v>174308427</v>
+        <v>113811</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B282">
-        <v>5696667314</v>
+        <v>174308427</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B283">
-        <v>38967</v>
+        <v>5696667314</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B284">
-        <v>3225166</v>
+        <v>38967</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B285">
-        <v>627988</v>
+        <v>3225166</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B286">
-        <v>4991</v>
+        <v>627988</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B287">
-        <v>1270630320</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B288">
-        <v>126860299</v>
+        <v>1270630320</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B289">
-        <v>747182815</v>
+        <v>126860299</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B290">
-        <v>366600944</v>
+        <v>747182815</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B291">
-        <v>29986262</v>
+        <v>366600944</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B292">
-        <v>36471766</v>
+        <v>29986262</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B293">
-        <v>30366043</v>
+        <v>36471766</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B294">
-        <v>54045422</v>
+        <v>30366043</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B295">
-        <v>2494524</v>
+        <v>54045422</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B296">
-        <v>10764</v>
+        <v>2494524</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B297">
-        <v>28608715</v>
+        <v>10764</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B298">
-        <v>17097123</v>
+        <v>28608715</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B299">
-        <v>17435228</v>
+        <v>17097123</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B300">
-        <v>282757</v>
+        <v>17435228</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B301">
-        <v>103923275</v>
+        <v>282757</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B302">
-        <v>4783062</v>
+        <v>103923275</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B303">
-        <v>4803553</v>
+        <v>4783062</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B304">
-        <v>6545503</v>
+        <v>4803553</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B305">
-        <v>23310719</v>
+        <v>6545503</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B306">
-        <v>200963603</v>
+        <v>23310719</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B307">
-        <v>1614</v>
+        <v>200963603</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B308">
-        <v>2907666</v>
+        <v>1614</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B309">
-        <v>1731701</v>
+        <v>2907666</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B310">
-        <v>494051484</v>
+        <v>1731701</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B311">
-        <v>940604181</v>
+        <v>494051484</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B312">
-        <v>2083458</v>
+        <v>940604181</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B313">
-        <v>241780765</v>
+        <v>2083458</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B314">
-        <v>517105558</v>
+        <v>241780765</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B315">
-        <v>366600944</v>
+        <v>517105558</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
@@ -4347,1289 +4353,1297 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B317">
-        <v>105768532</v>
+        <v>366600944</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B318">
-        <v>57213</v>
+        <v>105768532</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B319">
-        <v>5378859</v>
+        <v>57213</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B320">
-        <v>42128048</v>
+        <v>5378859</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B321">
-        <v>12141786</v>
+        <v>42128048</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B322">
-        <v>4974992</v>
+        <v>12141786</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B323">
-        <v>1307716642</v>
+        <v>4974992</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B324">
-        <v>1291387201</v>
+        <v>1307716642</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B325">
-        <v>1009950130</v>
+        <v>1291387201</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B326">
-        <v>507887773</v>
+        <v>1009950130</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B327">
-        <v>1872842323</v>
+        <v>507887773</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B328">
-        <v>216565317</v>
+        <v>1872842323</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B329">
-        <v>18001</v>
+        <v>216565317</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B330">
-        <v>4246440</v>
+        <v>18001</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B331">
-        <v>8776119</v>
+        <v>4246440</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B332">
-        <v>7044639</v>
+        <v>8776119</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B333">
-        <v>32510462</v>
+        <v>7044639</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B334">
-        <v>108116622</v>
+        <v>32510462</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B335">
-        <v>37887771</v>
+        <v>108116622</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B336">
-        <v>679769</v>
+        <v>37887771</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B337">
-        <v>10226178</v>
+        <v>679769</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B338">
-        <v>2933404</v>
+        <v>10226178</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B339">
-        <v>2832071</v>
+        <v>2933404</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B340">
-        <v>51225321</v>
+        <v>2832071</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B341">
-        <v>4043258</v>
+        <v>51225321</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B342">
-        <v>19364558</v>
+        <v>4043258</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B343">
-        <v>145872260</v>
+        <v>19364558</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B344">
-        <v>12626938</v>
+        <v>145872260</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B345">
-        <v>888932</v>
+        <v>12626938</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B346">
-        <v>15990784</v>
+        <v>888932</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B347">
-        <v>43309023</v>
+        <v>15990784</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B348">
-        <v>12129020</v>
+        <v>43309023</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B349">
-        <v>9853</v>
+        <v>12129020</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B350">
-        <v>6061</v>
+        <v>9853</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B351">
-        <v>52834</v>
+        <v>6061</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B352">
-        <v>182795</v>
+        <v>52834</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B353">
-        <v>38002</v>
+        <v>182795</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B354">
-        <v>5821</v>
+        <v>38002</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B355">
-        <v>110593</v>
+        <v>5821</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B356">
-        <v>197093</v>
+        <v>110593</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B357">
-        <v>33864</v>
+        <v>197093</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B358">
-        <v>215048</v>
+        <v>33864</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B359">
-        <v>34268529</v>
+        <v>215048</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B360">
-        <v>16296362</v>
+        <v>34268529</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B361">
-        <v>8772228</v>
+        <v>16296362</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B362">
-        <v>97741</v>
+        <v>8772228</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B363">
-        <v>3229909042</v>
+        <v>97741</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B364">
-        <v>7813207</v>
+        <v>3229909042</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B365">
-        <v>5804343</v>
+        <v>7813207</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B366">
-        <v>42389</v>
+        <v>5804343</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B367">
-        <v>5457012</v>
+        <v>42389</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B368">
-        <v>2078654</v>
+        <v>5457012</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B369">
-        <v>71428827</v>
+        <v>2078654</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B370">
-        <v>669821</v>
+        <v>71428827</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B371">
-        <v>15442906</v>
+        <v>669821</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B372">
-        <v>58558267</v>
+        <v>15442906</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B373">
-        <v>427199425</v>
+        <v>58558267</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B374">
-        <v>1835297503</v>
+        <v>427199425</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B375">
-        <v>11062114</v>
+        <v>1835297503</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B376">
-        <v>662011846</v>
+        <v>11062114</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B377">
-        <v>66629894</v>
+        <v>662011846</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B378">
-        <v>353940129</v>
+        <v>66629894</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B379">
-        <v>1918211396</v>
+        <v>353940129</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B380">
-        <v>306365495</v>
+        <v>1918211396</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B381">
-        <v>152446950</v>
+        <v>306365495</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B382">
-        <v>46736782</v>
+        <v>152446950</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B383">
-        <v>21323734</v>
+        <v>46736782</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B384">
-        <v>4981422</v>
+        <v>21323734</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B385">
-        <v>1066283411.0000001</v>
+        <v>4981422</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B386">
-        <v>42813237</v>
+        <v>1066283411.0000001</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B387">
-        <v>581363</v>
+        <v>42813237</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B388">
-        <v>10036391</v>
+        <v>581363</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B389">
-        <v>8591361</v>
+        <v>10036391</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B390">
-        <v>17070132</v>
+        <v>8591361</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B391">
-        <v>9321023</v>
+        <v>17070132</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B392">
-        <v>69625581</v>
+        <v>9321023</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B393">
-        <v>1293120</v>
+        <v>69625581</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B394">
-        <v>8082359</v>
+        <v>1293120</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B395">
-        <v>1330</v>
+        <v>8082359</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B396">
-        <v>104497</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B397">
-        <v>1394969</v>
+        <v>104497</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B398">
-        <v>11694721</v>
+        <v>1394969</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B399">
-        <v>83429607</v>
+        <v>11694721</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B400">
-        <v>5942094</v>
+        <v>83429607</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B401">
-        <v>38194</v>
+        <v>5942094</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B402">
-        <v>11655</v>
+        <v>38194</v>
       </c>
     </row>
     <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B403">
-        <v>1296680593</v>
+        <v>11655</v>
       </c>
     </row>
     <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B404">
-        <v>6358800278</v>
+        <v>1296680593</v>
       </c>
     </row>
     <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B405">
-        <v>370070433</v>
+        <v>6358800278</v>
       </c>
     </row>
     <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B406">
-        <v>4047949107</v>
+        <v>370070433</v>
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B407">
-        <v>601481415</v>
+        <v>4047949107</v>
       </c>
     </row>
     <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B408">
-        <v>248170834</v>
+        <v>601481415</v>
       </c>
     </row>
     <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B409">
-        <v>644001843</v>
+        <v>248170834</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B410">
-        <v>447126646</v>
+        <v>644001843</v>
       </c>
     </row>
     <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B411">
-        <v>6440543873</v>
+        <v>447126646</v>
       </c>
     </row>
     <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B412">
-        <v>2129737711.0000002</v>
+        <v>6440543873</v>
       </c>
     </row>
     <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B413">
-        <v>2397227</v>
+        <v>2129737711.0000002</v>
       </c>
     </row>
     <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B414">
-        <v>528864083</v>
+        <v>2397227</v>
       </c>
     </row>
     <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B415">
-        <v>279293796</v>
+        <v>528864083</v>
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B416">
-        <v>640775552</v>
+        <v>279293796</v>
       </c>
     </row>
     <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B417">
-        <v>643172779</v>
+        <v>640775552</v>
       </c>
     </row>
     <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B418">
-        <v>490260787</v>
+        <v>643172779</v>
       </c>
     </row>
     <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B419">
-        <v>1835297503</v>
+        <v>490260787</v>
       </c>
     </row>
     <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B420">
-        <v>533917214.00000006</v>
+        <v>1835297503</v>
       </c>
     </row>
     <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B421">
-        <v>7713468205</v>
+        <v>533917214.00000006</v>
       </c>
     </row>
     <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B422">
-        <v>2376751014</v>
+        <v>7713468205</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B423">
-        <v>425166056</v>
+        <v>2376751014</v>
       </c>
     </row>
     <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B424">
-        <v>575173373</v>
+        <v>425166056</v>
       </c>
     </row>
     <row r="425" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B425">
-        <v>922025316</v>
+        <v>575173373</v>
       </c>
     </row>
     <row r="426" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B426">
-        <v>648120956</v>
+        <v>922025316</v>
       </c>
     </row>
     <row r="427" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B427">
-        <v>455575824</v>
+        <v>648120956</v>
       </c>
     </row>
     <row r="428" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B428">
-        <v>366600944</v>
+        <v>455575824</v>
       </c>
     </row>
     <row r="429" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B429">
-        <v>1835297503</v>
+        <v>366600944</v>
       </c>
     </row>
     <row r="430" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B430">
-        <v>1109096648</v>
+        <v>1835297503</v>
       </c>
     </row>
     <row r="431" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B431">
-        <v>533923275</v>
+        <v>1109096648</v>
       </c>
     </row>
     <row r="432" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B432">
-        <v>496859260</v>
+        <v>533923275</v>
       </c>
     </row>
     <row r="433" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B433">
-        <v>7707903418</v>
+        <v>496859260</v>
       </c>
     </row>
     <row r="434" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B434">
-        <v>44269587</v>
+        <v>7707903418</v>
       </c>
     </row>
     <row r="435" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B435">
-        <v>43993643</v>
+        <v>44269587</v>
       </c>
     </row>
     <row r="436" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B436">
-        <v>9770526</v>
+        <v>43993643</v>
       </c>
     </row>
     <row r="437" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B437">
-        <v>67530161</v>
+        <v>9770526</v>
       </c>
     </row>
     <row r="438" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B438">
-        <v>68045699</v>
+        <v>67530161</v>
       </c>
     </row>
     <row r="439" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B439">
-        <v>1306320572</v>
+        <v>68045699</v>
       </c>
     </row>
     <row r="440" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B440">
-        <v>648117584</v>
+        <v>1306320572</v>
       </c>
     </row>
     <row r="441" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B441">
-        <v>4590691950</v>
+        <v>648117584</v>
       </c>
     </row>
     <row r="442" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B442">
-        <v>7707903510</v>
+        <v>4590691950</v>
       </c>
     </row>
     <row r="443" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A443" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B443">
-        <v>58005461</v>
+        <v>7707903510</v>
       </c>
     </row>
     <row r="444" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B444">
-        <v>104579</v>
+        <v>58005461</v>
       </c>
     </row>
     <row r="445" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B445">
-        <v>329064917</v>
+        <v>104579</v>
       </c>
     </row>
     <row r="446" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B446">
-        <v>332382720</v>
+        <v>329064917</v>
       </c>
     </row>
     <row r="447" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B447">
-        <v>2638958430</v>
+        <v>332382720</v>
       </c>
     </row>
     <row r="448" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B448">
-        <v>3461731</v>
+        <v>2638958430</v>
       </c>
     </row>
     <row r="449" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B449">
-        <v>32981714.999999996</v>
+        <v>3461731</v>
       </c>
     </row>
     <row r="450" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B450">
-        <v>299882</v>
+        <v>32981714.999999996</v>
       </c>
     </row>
     <row r="451" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B451">
-        <v>28515829</v>
+        <v>299882</v>
       </c>
     </row>
     <row r="452" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B452">
-        <v>96462108</v>
+        <v>28515829</v>
       </c>
     </row>
     <row r="453" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B453">
-        <v>2129754531</v>
+        <v>96462108</v>
       </c>
     </row>
     <row r="454" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B454">
-        <v>421035757</v>
+        <v>2129754531</v>
       </c>
     </row>
     <row r="455" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B455">
-        <v>569811869</v>
+        <v>421035757</v>
       </c>
     </row>
     <row r="456" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B456">
-        <v>389753191</v>
+        <v>569811869</v>
       </c>
     </row>
     <row r="457" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B457">
-        <v>1835297503</v>
+        <v>389753191</v>
       </c>
     </row>
     <row r="458" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B458">
-        <v>1106864204</v>
+        <v>1835297503</v>
       </c>
     </row>
     <row r="459" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B459">
-        <v>7668888226</v>
+        <v>1106864204</v>
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B460">
-        <v>1091758856</v>
+        <v>7668888226</v>
       </c>
     </row>
     <row r="461" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B461">
-        <v>1009950130</v>
+        <v>1091758856</v>
       </c>
     </row>
     <row r="462" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B462">
-        <v>712276291</v>
+        <v>1009950130</v>
       </c>
     </row>
     <row r="463" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B463">
-        <v>930166618</v>
+        <v>712276291</v>
       </c>
     </row>
     <row r="464" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B464">
-        <v>2001946277</v>
+        <v>930166618</v>
       </c>
     </row>
     <row r="465" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A465" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B465">
-        <v>1922790054</v>
+        <v>2001946277</v>
       </c>
     </row>
     <row r="466" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A466" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B466">
-        <v>11436</v>
+        <v>1922790054</v>
       </c>
     </row>
     <row r="467" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A467" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B467">
-        <v>127107468</v>
+        <v>11436</v>
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B468">
-        <v>391440147</v>
+        <v>127107468</v>
       </c>
     </row>
     <row r="469" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B469">
-        <v>275324793</v>
+        <v>391440147</v>
       </c>
     </row>
     <row r="470" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B470">
-        <v>195522412</v>
+        <v>275324793</v>
       </c>
     </row>
     <row r="471" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B471">
-        <v>919088423</v>
+        <v>195522412</v>
       </c>
     </row>
     <row r="472" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B472">
-        <v>582458</v>
+        <v>919088423</v>
       </c>
     </row>
     <row r="473" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A473" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B473">
-        <v>7713468205</v>
+        <v>582458</v>
       </c>
     </row>
     <row r="474" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B474">
-        <v>6452517055</v>
+        <v>7713468205</v>
       </c>
     </row>
     <row r="475" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B475">
-        <v>29161922</v>
+        <v>6452517055</v>
       </c>
     </row>
     <row r="476" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B476">
-        <v>17861034</v>
+        <v>29161922</v>
       </c>
     </row>
     <row r="477" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
+        <v>470</v>
+      </c>
+      <c r="B477">
+        <v>17861034</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A478" t="s">
         <v>471</v>
       </c>
-      <c r="B477">
+      <c r="B478">
         <v>14645473</v>
       </c>
     </row>

</xml_diff>